<commit_message>
- Minor edits made while batch tracking latest larval schooling dataset.
</commit_message>
<xml_diff>
--- a/settings/larval-schooling-2.xlsx
+++ b/settings/larval-schooling-2.xlsx
@@ -243,10 +243,10 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.11"/>
@@ -401,7 +401,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2"/>
     </row>

</xml_diff>